<commit_message>
Various updates associated with merge
</commit_message>
<xml_diff>
--- a/tabular/references/reference_feature_locations.xlsx
+++ b/tabular/references/reference_feature_locations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="0" windowWidth="18940" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="27340" yWindow="3200" windowWidth="18940" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,25 +43,7 @@
     <t>VP</t>
   </si>
   <si>
-    <t>CPV</t>
-  </si>
-  <si>
     <t>5UTR</t>
-  </si>
-  <si>
-    <t>MVM1</t>
-  </si>
-  <si>
-    <t>PPV</t>
-  </si>
-  <si>
-    <t>MpBuV</t>
-  </si>
-  <si>
-    <t>AMDV</t>
-  </si>
-  <si>
-    <t>ChPV</t>
   </si>
   <si>
     <t>MVC</t>
@@ -70,49 +52,67 @@
     <t>Mid-ORF</t>
   </si>
   <si>
-    <t>BPV</t>
-  </si>
-  <si>
-    <t>PBoV</t>
-  </si>
-  <si>
-    <t>CMV</t>
-  </si>
-  <si>
-    <t>AAV2</t>
-  </si>
-  <si>
-    <t>CAV</t>
-  </si>
-  <si>
-    <t>GPV</t>
-  </si>
-  <si>
-    <t>MDPV</t>
-  </si>
-  <si>
-    <t>B19</t>
-  </si>
-  <si>
-    <t>BPV2</t>
-  </si>
-  <si>
-    <t>SnakePV</t>
-  </si>
-  <si>
-    <t>HamsterPV</t>
-  </si>
-  <si>
     <t>M</t>
-  </si>
-  <si>
-    <t>Mk-PV</t>
   </si>
   <si>
     <t>NS2-L</t>
   </si>
   <si>
     <t>NS2-P</t>
+  </si>
+  <si>
+    <t>REF_CPV</t>
+  </si>
+  <si>
+    <t>REF_MVM1</t>
+  </si>
+  <si>
+    <t>REF_PPV</t>
+  </si>
+  <si>
+    <t>REF_MpBuV</t>
+  </si>
+  <si>
+    <t>REF_AMDV</t>
+  </si>
+  <si>
+    <t>REF_ChPV</t>
+  </si>
+  <si>
+    <t>REF_BPV</t>
+  </si>
+  <si>
+    <t>REF_PBoV</t>
+  </si>
+  <si>
+    <t>REF_CMV</t>
+  </si>
+  <si>
+    <t>REF_AAV2</t>
+  </si>
+  <si>
+    <t>REF_SnakePV</t>
+  </si>
+  <si>
+    <t>REF_CAV</t>
+  </si>
+  <si>
+    <t>REF_GPV</t>
+  </si>
+  <si>
+    <t>REF_MDPV</t>
+  </si>
+  <si>
+    <t>REF_B19</t>
+  </si>
+  <si>
+    <t>REF_BPV2</t>
+  </si>
+  <si>
+    <t>REF_HamsterPV</t>
+  </si>
+  <si>
+    <t>REF_Mk-PV</t>
   </si>
 </sst>
 </file>
@@ -125,6 +125,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -193,9 +194,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1639">
+  <cellStyleXfs count="1643">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1843,7 +1848,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1639">
+  <cellStyles count="1643">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2664,6 +2669,8 @@
     <cellStyle name="Followed Hyperlink" xfId="1634" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1636" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1642" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -3482,6 +3489,8 @@
     <cellStyle name="Hyperlink" xfId="1633" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1635" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1641" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3818,8 +3827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1500"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D43" sqref="A1:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3849,10 +3858,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -3863,7 +3872,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>4</v>
@@ -3877,7 +3886,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -3891,7 +3900,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>4</v>
@@ -3905,7 +3914,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>5</v>
@@ -3919,7 +3928,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -3933,7 +3942,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>5</v>
@@ -3947,7 +3956,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -3961,7 +3970,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>5</v>
@@ -3975,7 +3984,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
@@ -3989,7 +3998,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>5</v>
@@ -4003,7 +4012,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
@@ -4017,7 +4026,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>5</v>
@@ -4031,7 +4040,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>4</v>
@@ -4045,10 +4054,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C16" s="5">
         <v>2661</v>
@@ -4059,7 +4068,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>5</v>
@@ -4073,7 +4082,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>4</v>
@@ -4087,10 +4096,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C19" s="5">
         <v>2333</v>
@@ -4101,7 +4110,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>5</v>
@@ -4115,7 +4124,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>4</v>
@@ -4129,10 +4138,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C22" s="5">
         <v>2389</v>
@@ -4143,7 +4152,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>5</v>
@@ -4157,7 +4166,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>4</v>
@@ -4171,7 +4180,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>5</v>
@@ -4185,7 +4194,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>4</v>
@@ -4199,7 +4208,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>5</v>
@@ -4213,7 +4222,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>4</v>
@@ -4227,7 +4236,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>5</v>
@@ -4241,7 +4250,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>4</v>
@@ -4255,7 +4264,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>5</v>
@@ -4269,7 +4278,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>4</v>
@@ -4283,7 +4292,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>5</v>
@@ -4297,7 +4306,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>4</v>
@@ -4311,7 +4320,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>5</v>
@@ -4325,7 +4334,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>4</v>
@@ -4339,7 +4348,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>5</v>
@@ -4353,7 +4362,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>4</v>
@@ -4367,7 +4376,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>5</v>
@@ -4381,10 +4390,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C40" s="5">
         <v>219</v>
@@ -4395,7 +4404,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>4</v>
@@ -4409,10 +4418,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C42" s="5">
         <v>2006</v>
@@ -4423,7 +4432,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>5</v>
@@ -5099,7 +5108,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -5113,10 +5122,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>2661</v>
@@ -5127,7 +5136,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Creating minimal, systematically named alignment file set
</commit_message>
<xml_diff>
--- a/tabular/references/reference_feature_locations.xlsx
+++ b/tabular/references/reference_feature_locations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="36">
   <si>
     <t>referenceName</t>
   </si>
@@ -114,6 +114,24 @@
   <si>
     <t>REF_Mk-PV</t>
   </si>
+  <si>
+    <t>REF_AAV3</t>
+  </si>
+  <si>
+    <t>REF_AAV4</t>
+  </si>
+  <si>
+    <t>REF_AAV5</t>
+  </si>
+  <si>
+    <t>REF_AAV6</t>
+  </si>
+  <si>
+    <t>REF_AAV7</t>
+  </si>
+  <si>
+    <t>REF_AAV8</t>
+  </si>
 </sst>
 </file>
 
@@ -165,7 +183,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +202,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -194,7 +218,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1645">
+  <cellStyleXfs count="1661">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1840,8 +1864,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1849,8 +1889,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1645">
+  <cellStyles count="1661">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2674,6 +2730,14 @@
     <cellStyle name="Followed Hyperlink" xfId="1640" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1642" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1660" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -3495,6 +3559,14 @@
     <cellStyle name="Hyperlink" xfId="1639" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1641" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1659" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3829,18 +3901,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1500"/>
+  <dimension ref="A1:E1512"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12" style="11" customWidth="1"/>
     <col min="5" max="5" width="31.83203125" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
@@ -3853,10 +3925,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3870,7 +3942,7 @@
       <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="9">
         <v>130</v>
       </c>
     </row>
@@ -3884,7 +3956,7 @@
       <c r="C3" s="5">
         <v>130</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="9">
         <v>465</v>
       </c>
     </row>
@@ -3898,7 +3970,7 @@
       <c r="C4" s="5">
         <v>466</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="9">
         <v>969</v>
       </c>
     </row>
@@ -3912,7 +3984,7 @@
       <c r="C5" s="5">
         <v>114</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="9">
         <v>2279</v>
       </c>
     </row>
@@ -3926,7 +3998,7 @@
       <c r="C6" s="5">
         <v>2399</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="9">
         <v>4555</v>
       </c>
     </row>
@@ -3940,7 +4012,7 @@
       <c r="C7" s="5">
         <v>292</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="9">
         <v>2280</v>
       </c>
     </row>
@@ -3954,7 +4026,7 @@
       <c r="C8" s="5">
         <v>2388</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="10">
         <v>4547</v>
       </c>
     </row>
@@ -3968,7 +4040,7 @@
       <c r="C9" s="5">
         <v>63</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="9">
         <v>1982</v>
       </c>
     </row>
@@ -3982,7 +4054,7 @@
       <c r="C10" s="5">
         <v>2247</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="9">
         <v>4403</v>
       </c>
     </row>
@@ -3996,7 +4068,7 @@
       <c r="C11" s="5">
         <v>206</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="9">
         <v>1978</v>
       </c>
     </row>
@@ -4010,7 +4082,7 @@
       <c r="C12" s="5">
         <v>2406</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="9">
         <v>4349</v>
       </c>
     </row>
@@ -4024,7 +4096,7 @@
       <c r="C13" s="5">
         <v>411</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="9">
         <v>2495</v>
       </c>
     </row>
@@ -4038,7 +4110,7 @@
       <c r="C14" s="5">
         <v>2998</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="9">
         <v>5025</v>
       </c>
     </row>
@@ -4052,7 +4124,7 @@
       <c r="C15" s="5">
         <v>740</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="9">
         <v>2920</v>
       </c>
     </row>
@@ -4066,7 +4138,7 @@
       <c r="C16" s="5">
         <v>2661</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="9">
         <v>3302</v>
       </c>
     </row>
@@ -4080,7 +4152,7 @@
       <c r="C17" s="5">
         <v>3286</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="9">
         <v>5307</v>
       </c>
     </row>
@@ -4094,7 +4166,7 @@
       <c r="C18" s="5">
         <v>149</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="9">
         <v>2260</v>
       </c>
     </row>
@@ -4108,7 +4180,7 @@
       <c r="C19" s="5">
         <v>2333</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="9">
         <v>3019</v>
       </c>
     </row>
@@ -4122,7 +4194,7 @@
       <c r="C20" s="5">
         <v>3003</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="9">
         <v>5120</v>
       </c>
     </row>
@@ -4136,7 +4208,7 @@
       <c r="C21" s="5">
         <v>429</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="9">
         <v>2579</v>
       </c>
     </row>
@@ -4150,7 +4222,7 @@
       <c r="C22" s="5">
         <v>2389</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="9">
         <v>2949</v>
       </c>
     </row>
@@ -4164,7 +4236,7 @@
       <c r="C23" s="5">
         <v>2933</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="9">
         <v>5044</v>
       </c>
     </row>
@@ -4178,7 +4250,7 @@
       <c r="C24" s="5">
         <v>321</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="9">
         <v>2252</v>
       </c>
     </row>
@@ -4192,382 +4264,502 @@
       <c r="C25" s="5">
         <v>2203</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="9">
         <v>4410</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="5">
-        <v>324</v>
-      </c>
-      <c r="D26" s="5">
-        <v>2012</v>
+        <v>318</v>
+      </c>
+      <c r="D26" s="9">
+        <v>2192</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="5">
-        <v>2030</v>
-      </c>
-      <c r="D27" s="5">
-        <v>4210</v>
+        <v>2209</v>
+      </c>
+      <c r="D27" s="9">
+        <v>4419</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="5">
-        <v>347</v>
-      </c>
-      <c r="D28" s="5">
-        <v>2179</v>
+        <v>372</v>
+      </c>
+      <c r="D28" s="9">
+        <v>2243</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="5">
-        <v>2195</v>
-      </c>
-      <c r="D29" s="5">
-        <v>4375</v>
+        <v>2260</v>
+      </c>
+      <c r="D29" s="9">
+        <v>4464</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="5">
-        <v>537</v>
-      </c>
-      <c r="D30" s="5">
-        <v>2420</v>
+        <v>359</v>
+      </c>
+      <c r="D30" s="9">
+        <v>2191</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="5">
-        <v>2439</v>
-      </c>
-      <c r="D31" s="5">
-        <v>4637</v>
+        <v>2207</v>
+      </c>
+      <c r="D31" s="9">
+        <v>4381</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="5">
-        <v>548</v>
-      </c>
-      <c r="D32" s="5">
-        <v>2431</v>
+        <v>320</v>
+      </c>
+      <c r="D32" s="9">
+        <v>2191</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="5" t="s">
+      <c r="A33" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="5">
-        <v>2450</v>
-      </c>
-      <c r="D33" s="5">
-        <v>4648</v>
+        <v>2208</v>
+      </c>
+      <c r="D33" s="9">
+        <v>4418</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="5">
-        <v>616</v>
-      </c>
-      <c r="D34" s="5">
-        <v>2631</v>
+        <v>334</v>
+      </c>
+      <c r="D34" s="9">
+        <v>2205</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="5">
-        <v>2624</v>
-      </c>
-      <c r="D35" s="5">
-        <v>4969</v>
+        <v>2222</v>
+      </c>
+      <c r="D35" s="9">
+        <v>4435</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="5">
-        <v>306</v>
-      </c>
-      <c r="D36" s="5">
-        <v>1919</v>
+        <v>227</v>
+      </c>
+      <c r="D36" s="9">
+        <v>2104</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="5">
-        <v>2268</v>
-      </c>
-      <c r="D37" s="5">
-        <v>5384</v>
+        <v>2121</v>
+      </c>
+      <c r="D37" s="9">
+        <v>4337</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C38" s="5">
-        <v>122</v>
-      </c>
-      <c r="D38" s="5">
-        <v>2140</v>
+        <v>324</v>
+      </c>
+      <c r="D38" s="9">
+        <v>2012</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="5">
-        <v>2664</v>
-      </c>
-      <c r="D39" s="5">
-        <v>4427</v>
+        <v>2030</v>
+      </c>
+      <c r="D39" s="9">
+        <v>4210</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="6" t="s">
-        <v>29</v>
+      <c r="A40" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C40" s="5">
-        <v>2109</v>
-      </c>
-      <c r="D40" s="5">
-        <v>2728</v>
+        <v>347</v>
+      </c>
+      <c r="D40" s="9">
+        <v>2179</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="6" t="s">
-        <v>29</v>
+      <c r="A41" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="5">
+        <v>2195</v>
+      </c>
+      <c r="D41" s="9">
+        <v>4375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="5">
-        <v>811</v>
-      </c>
-      <c r="D41" s="5">
-        <v>2790</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="C42" s="5">
-        <v>2006</v>
-      </c>
-      <c r="D42" s="5">
-        <v>2726</v>
+        <v>537</v>
+      </c>
+      <c r="D42" s="9">
+        <v>2420</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="6" t="s">
-        <v>29</v>
+      <c r="A43" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="5">
+        <v>2439</v>
+      </c>
+      <c r="D43" s="9">
+        <v>4637</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="5">
+        <v>548</v>
+      </c>
+      <c r="D44" s="9">
+        <v>2431</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="5">
+        <v>2450</v>
+      </c>
+      <c r="D45" s="9">
+        <v>4648</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="5">
+        <v>616</v>
+      </c>
+      <c r="D46" s="9">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="5">
+        <v>2624</v>
+      </c>
+      <c r="D47" s="9">
+        <v>4969</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="5">
+        <v>306</v>
+      </c>
+      <c r="D48" s="9">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="5">
+        <v>2268</v>
+      </c>
+      <c r="D49" s="9">
+        <v>5384</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="5">
+        <v>122</v>
+      </c>
+      <c r="D50" s="9">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="5">
+        <v>2664</v>
+      </c>
+      <c r="D51" s="9">
+        <v>4427</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="5">
+        <v>2109</v>
+      </c>
+      <c r="D52" s="9">
+        <v>2728</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="5">
+        <v>811</v>
+      </c>
+      <c r="D53" s="9">
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="5">
+        <v>2006</v>
+      </c>
+      <c r="D54" s="9">
+        <v>2726</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="5">
         <v>2783</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D55" s="9">
         <v>4273</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="14" customHeight="1"/>
-    <row r="54" spans="2:2">
-      <c r="B54" s="4"/>
-    </row>
-    <row r="59" spans="2:2" ht="16" customHeight="1"/>
-    <row r="68" spans="1:4">
-      <c r="A68" s="2"/>
-      <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="2"/>
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="2"/>
-      <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="2"/>
-      <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="2"/>
-      <c r="B72" s="1"/>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="2"/>
-      <c r="B73" s="1"/>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="2"/>
-      <c r="B74" s="1"/>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="2"/>
-      <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="2"/>
-      <c r="B76" s="1"/>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="2"/>
-      <c r="B77" s="1"/>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="2"/>
-      <c r="B78" s="1"/>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="2"/>
-      <c r="B79" s="1"/>
-    </row>
-    <row r="80" spans="1:4">
+    <row r="65" spans="1:2" ht="14" customHeight="1"/>
+    <row r="66" spans="1:2">
+      <c r="B66" s="4"/>
+    </row>
+    <row r="71" spans="1:2" ht="16" customHeight="1"/>
+    <row r="80" spans="1:2">
       <c r="A80" s="2"/>
       <c r="B80" s="1"/>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:4">
       <c r="A81" s="2"/>
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:4">
       <c r="A82" s="2"/>
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:4">
       <c r="A83" s="2"/>
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:4">
       <c r="A84" s="2"/>
       <c r="B84" s="1"/>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:4">
       <c r="A85" s="2"/>
       <c r="B85" s="1"/>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:4">
       <c r="A86" s="2"/>
       <c r="B86" s="1"/>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:4">
       <c r="A87" s="2"/>
       <c r="B87" s="1"/>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:4">
       <c r="A88" s="2"/>
       <c r="B88" s="1"/>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:4">
       <c r="A89" s="2"/>
       <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="D89" s="12"/>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="2"/>
       <c r="B90" s="1"/>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="D90" s="12"/>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" s="2"/>
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:4">
       <c r="A92" s="2"/>
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:4">
       <c r="A93" s="2"/>
       <c r="B93" s="1"/>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:4">
       <c r="A94" s="2"/>
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:4">
       <c r="A95" s="2"/>
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:4">
       <c r="A96" s="2"/>
       <c r="B96" s="1"/>
     </row>
@@ -4582,7 +4774,6 @@
     <row r="99" spans="1:3">
       <c r="A99" s="2"/>
       <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="2"/>
@@ -4602,6 +4793,7 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="2"/>
+      <c r="B104" s="1"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="2"/>
@@ -4630,6 +4822,7 @@
     <row r="111" spans="1:3">
       <c r="A111" s="2"/>
       <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="2"/>
@@ -4638,21 +4831,17 @@
     <row r="113" spans="1:5">
       <c r="A113" s="2"/>
       <c r="B113" s="1"/>
-      <c r="E113" s="2"/>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="2"/>
       <c r="B114" s="1"/>
-      <c r="E114" s="2"/>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="2"/>
       <c r="B115" s="1"/>
-      <c r="E115" s="2"/>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="2"/>
-      <c r="B116" s="1"/>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="2"/>
@@ -4689,14 +4878,17 @@
     <row r="125" spans="1:5">
       <c r="A125" s="2"/>
       <c r="B125" s="1"/>
+      <c r="E125" s="2"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="2"/>
       <c r="B126" s="1"/>
+      <c r="E126" s="2"/>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="2"/>
       <c r="B127" s="1"/>
+      <c r="E127" s="2"/>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="2"/>
@@ -4774,71 +4966,71 @@
       <c r="A146" s="2"/>
       <c r="B146" s="1"/>
     </row>
-    <row r="164" spans="5:5">
-      <c r="E164" s="1"/>
-    </row>
-    <row r="165" spans="5:5">
-      <c r="E165" s="1"/>
-    </row>
-    <row r="166" spans="5:5">
-      <c r="E166" s="1"/>
-    </row>
-    <row r="167" spans="5:5">
-      <c r="E167" s="1"/>
-    </row>
-    <row r="168" spans="5:5">
-      <c r="E168" s="1"/>
-    </row>
-    <row r="169" spans="5:5">
-      <c r="E169" s="1"/>
-    </row>
-    <row r="222" spans="1:2">
-      <c r="A222" s="2"/>
-      <c r="B222" s="1"/>
-    </row>
-    <row r="223" spans="1:2">
-      <c r="A223" s="2"/>
-      <c r="B223" s="1"/>
-    </row>
-    <row r="224" spans="1:2">
-      <c r="A224" s="2"/>
-      <c r="B224" s="1"/>
-    </row>
-    <row r="225" spans="1:2">
-      <c r="A225" s="2"/>
-      <c r="B225" s="1"/>
-    </row>
-    <row r="226" spans="1:2">
-      <c r="A226" s="2"/>
-      <c r="B226" s="1"/>
-    </row>
-    <row r="227" spans="1:2">
-      <c r="A227" s="2"/>
-      <c r="B227" s="1"/>
-    </row>
-    <row r="228" spans="1:2">
-      <c r="A228" s="2"/>
-      <c r="B228" s="1"/>
-    </row>
-    <row r="229" spans="1:2">
-      <c r="A229" s="2"/>
-      <c r="B229" s="1"/>
-    </row>
-    <row r="230" spans="1:2">
-      <c r="A230" s="2"/>
-      <c r="B230" s="1"/>
-    </row>
-    <row r="231" spans="1:2">
-      <c r="A231" s="2"/>
-      <c r="B231" s="1"/>
-    </row>
-    <row r="232" spans="1:2">
-      <c r="A232" s="2"/>
-      <c r="B232" s="1"/>
-    </row>
-    <row r="233" spans="1:2">
-      <c r="A233" s="2"/>
-      <c r="B233" s="1"/>
+    <row r="147" spans="1:2">
+      <c r="A147" s="2"/>
+      <c r="B147" s="1"/>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="2"/>
+      <c r="B148" s="1"/>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="2"/>
+      <c r="B149" s="1"/>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="2"/>
+      <c r="B150" s="1"/>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="2"/>
+      <c r="B151" s="1"/>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="2"/>
+      <c r="B152" s="1"/>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="2"/>
+      <c r="B153" s="1"/>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="2"/>
+      <c r="B154" s="1"/>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="2"/>
+      <c r="B155" s="1"/>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="2"/>
+      <c r="B156" s="1"/>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="2"/>
+      <c r="B157" s="1"/>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="2"/>
+      <c r="B158" s="1"/>
+    </row>
+    <row r="176" spans="5:5">
+      <c r="E176" s="1"/>
+    </row>
+    <row r="177" spans="5:5">
+      <c r="E177" s="1"/>
+    </row>
+    <row r="178" spans="5:5">
+      <c r="E178" s="1"/>
+    </row>
+    <row r="179" spans="5:5">
+      <c r="E179" s="1"/>
+    </row>
+    <row r="180" spans="5:5">
+      <c r="E180" s="1"/>
+    </row>
+    <row r="181" spans="5:5">
+      <c r="E181" s="1"/>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="2"/>
@@ -4890,6 +5082,7 @@
     </row>
     <row r="246" spans="1:2">
       <c r="A246" s="2"/>
+      <c r="B246" s="1"/>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" s="2"/>
@@ -4919,92 +5112,106 @@
       <c r="A253" s="2"/>
       <c r="B253" s="1"/>
     </row>
-    <row r="936" spans="3:3">
-      <c r="C936" s="2"/>
-    </row>
-    <row r="1072" spans="1:1">
-      <c r="A1072" s="2"/>
-    </row>
-    <row r="1073" spans="1:1">
-      <c r="A1073" s="2"/>
-    </row>
-    <row r="1198" spans="1:1">
-      <c r="A1198" s="2"/>
-    </row>
-    <row r="1199" spans="1:1">
-      <c r="A1199" s="2"/>
-    </row>
-    <row r="1200" spans="1:1">
-      <c r="A1200" s="2"/>
-    </row>
-    <row r="1201" spans="1:1">
-      <c r="A1201" s="2"/>
-    </row>
-    <row r="1202" spans="1:1">
-      <c r="A1202" s="2"/>
-    </row>
-    <row r="1203" spans="1:1">
-      <c r="A1203" s="2"/>
-    </row>
-    <row r="1248" spans="3:4">
-      <c r="C1248" s="2"/>
-      <c r="D1248" s="2"/>
-    </row>
-    <row r="1249" spans="1:4">
-      <c r="C1249" s="2"/>
-      <c r="D1249" s="2"/>
-    </row>
-    <row r="1250" spans="1:4">
-      <c r="C1250" s="2"/>
-      <c r="D1250" s="2"/>
-    </row>
-    <row r="1252" spans="1:4">
-      <c r="A1252" s="2"/>
-    </row>
-    <row r="1253" spans="1:4">
-      <c r="A1253" s="2"/>
-    </row>
-    <row r="1254" spans="1:4">
-      <c r="A1254" s="2"/>
-    </row>
-    <row r="1255" spans="1:4">
-      <c r="A1255" s="2"/>
-    </row>
-    <row r="1256" spans="1:4">
-      <c r="A1256" s="2"/>
-    </row>
-    <row r="1275" spans="1:1">
-      <c r="A1275" s="2"/>
-    </row>
-    <row r="1276" spans="1:1">
-      <c r="A1276" s="2"/>
-    </row>
-    <row r="1277" spans="1:1">
-      <c r="A1277" s="2"/>
-    </row>
-    <row r="1278" spans="1:1">
-      <c r="A1278" s="2"/>
-    </row>
-    <row r="1279" spans="1:1">
-      <c r="A1279" s="2"/>
-    </row>
-    <row r="1280" spans="1:1">
-      <c r="A1280" s="2"/>
-    </row>
-    <row r="1281" spans="1:1">
-      <c r="A1281" s="2"/>
-    </row>
-    <row r="1283" spans="1:1">
-      <c r="A1283" s="2"/>
-    </row>
-    <row r="1284" spans="1:1">
-      <c r="A1284" s="2"/>
-    </row>
-    <row r="1285" spans="1:1">
-      <c r="A1285" s="2"/>
-    </row>
-    <row r="1286" spans="1:1">
-      <c r="A1286" s="2"/>
+    <row r="254" spans="1:2">
+      <c r="A254" s="2"/>
+      <c r="B254" s="1"/>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="A255" s="2"/>
+      <c r="B255" s="1"/>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256" s="2"/>
+      <c r="B256" s="1"/>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257" s="2"/>
+      <c r="B257" s="1"/>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258" s="2"/>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" s="2"/>
+      <c r="B259" s="1"/>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260" s="2"/>
+      <c r="B260" s="1"/>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="A261" s="2"/>
+      <c r="B261" s="1"/>
+    </row>
+    <row r="262" spans="1:2">
+      <c r="A262" s="2"/>
+      <c r="B262" s="1"/>
+    </row>
+    <row r="263" spans="1:2">
+      <c r="A263" s="2"/>
+      <c r="B263" s="1"/>
+    </row>
+    <row r="264" spans="1:2">
+      <c r="A264" s="2"/>
+      <c r="B264" s="1"/>
+    </row>
+    <row r="265" spans="1:2">
+      <c r="A265" s="2"/>
+      <c r="B265" s="1"/>
+    </row>
+    <row r="948" spans="3:3">
+      <c r="C948" s="2"/>
+    </row>
+    <row r="1084" spans="1:1">
+      <c r="A1084" s="2"/>
+    </row>
+    <row r="1085" spans="1:1">
+      <c r="A1085" s="2"/>
+    </row>
+    <row r="1210" spans="1:1">
+      <c r="A1210" s="2"/>
+    </row>
+    <row r="1211" spans="1:1">
+      <c r="A1211" s="2"/>
+    </row>
+    <row r="1212" spans="1:1">
+      <c r="A1212" s="2"/>
+    </row>
+    <row r="1213" spans="1:1">
+      <c r="A1213" s="2"/>
+    </row>
+    <row r="1214" spans="1:1">
+      <c r="A1214" s="2"/>
+    </row>
+    <row r="1215" spans="1:1">
+      <c r="A1215" s="2"/>
+    </row>
+    <row r="1260" spans="1:4">
+      <c r="C1260" s="2"/>
+      <c r="D1260" s="12"/>
+    </row>
+    <row r="1261" spans="1:4">
+      <c r="C1261" s="2"/>
+      <c r="D1261" s="12"/>
+    </row>
+    <row r="1262" spans="1:4">
+      <c r="C1262" s="2"/>
+      <c r="D1262" s="12"/>
+    </row>
+    <row r="1264" spans="1:4">
+      <c r="A1264" s="2"/>
+    </row>
+    <row r="1265" spans="1:1">
+      <c r="A1265" s="2"/>
+    </row>
+    <row r="1266" spans="1:1">
+      <c r="A1266" s="2"/>
+    </row>
+    <row r="1267" spans="1:1">
+      <c r="A1267" s="2"/>
+    </row>
+    <row r="1268" spans="1:1">
+      <c r="A1268" s="2"/>
     </row>
     <row r="1287" spans="1:1">
       <c r="A1287" s="2"/>
@@ -5012,82 +5219,115 @@
     <row r="1288" spans="1:1">
       <c r="A1288" s="2"/>
     </row>
-    <row r="1340" spans="1:1">
-      <c r="A1340" s="2"/>
-    </row>
-    <row r="1341" spans="1:1">
-      <c r="A1341" s="2"/>
-    </row>
-    <row r="1342" spans="1:1">
-      <c r="A1342" s="2"/>
-    </row>
-    <row r="1343" spans="1:1">
-      <c r="A1343" s="2"/>
-    </row>
-    <row r="1345" spans="1:1">
-      <c r="A1345" s="2"/>
-    </row>
-    <row r="1346" spans="1:1">
-      <c r="A1346" s="2"/>
-    </row>
-    <row r="1347" spans="1:1">
-      <c r="A1347" s="2"/>
-    </row>
-    <row r="1348" spans="1:1">
-      <c r="A1348" s="2"/>
-    </row>
-    <row r="1383" spans="1:1">
-      <c r="A1383" s="2"/>
-    </row>
-    <row r="1384" spans="1:1">
-      <c r="A1384" s="2"/>
-    </row>
-    <row r="1385" spans="1:1">
-      <c r="A1385" s="2"/>
-    </row>
-    <row r="1386" spans="1:1">
-      <c r="A1386" s="2"/>
-    </row>
-    <row r="1387" spans="1:1">
-      <c r="A1387" s="2"/>
-    </row>
-    <row r="1388" spans="1:1">
-      <c r="A1388" s="2"/>
-    </row>
-    <row r="1430" spans="2:4">
-      <c r="C1430" s="2"/>
-      <c r="D1430" s="2"/>
-    </row>
-    <row r="1431" spans="2:4">
-      <c r="B1431" s="2"/>
-      <c r="C1431" s="2"/>
-      <c r="D1431" s="2"/>
-    </row>
-    <row r="1432" spans="2:4">
-      <c r="B1432" s="2"/>
-      <c r="C1432" s="2"/>
-      <c r="D1432" s="2"/>
-    </row>
-    <row r="1433" spans="2:4">
-      <c r="B1433" s="2"/>
-      <c r="C1433" s="2"/>
-      <c r="D1433" s="2"/>
-    </row>
-    <row r="1434" spans="2:4">
-      <c r="C1434" s="2"/>
-      <c r="D1434" s="2"/>
-    </row>
-    <row r="1497" spans="1:1">
-      <c r="A1497" s="2"/>
-    </row>
-    <row r="1498" spans="1:1">
-      <c r="A1498" s="2"/>
-    </row>
-    <row r="1499" spans="1:1">
-      <c r="A1499" s="2"/>
-    </row>
-    <row r="1500" spans="1:1">
-      <c r="A1500" s="2"/>
+    <row r="1289" spans="1:1">
+      <c r="A1289" s="2"/>
+    </row>
+    <row r="1290" spans="1:1">
+      <c r="A1290" s="2"/>
+    </row>
+    <row r="1291" spans="1:1">
+      <c r="A1291" s="2"/>
+    </row>
+    <row r="1292" spans="1:1">
+      <c r="A1292" s="2"/>
+    </row>
+    <row r="1293" spans="1:1">
+      <c r="A1293" s="2"/>
+    </row>
+    <row r="1295" spans="1:1">
+      <c r="A1295" s="2"/>
+    </row>
+    <row r="1296" spans="1:1">
+      <c r="A1296" s="2"/>
+    </row>
+    <row r="1297" spans="1:1">
+      <c r="A1297" s="2"/>
+    </row>
+    <row r="1298" spans="1:1">
+      <c r="A1298" s="2"/>
+    </row>
+    <row r="1299" spans="1:1">
+      <c r="A1299" s="2"/>
+    </row>
+    <row r="1300" spans="1:1">
+      <c r="A1300" s="2"/>
+    </row>
+    <row r="1352" spans="1:1">
+      <c r="A1352" s="2"/>
+    </row>
+    <row r="1353" spans="1:1">
+      <c r="A1353" s="2"/>
+    </row>
+    <row r="1354" spans="1:1">
+      <c r="A1354" s="2"/>
+    </row>
+    <row r="1355" spans="1:1">
+      <c r="A1355" s="2"/>
+    </row>
+    <row r="1357" spans="1:1">
+      <c r="A1357" s="2"/>
+    </row>
+    <row r="1358" spans="1:1">
+      <c r="A1358" s="2"/>
+    </row>
+    <row r="1359" spans="1:1">
+      <c r="A1359" s="2"/>
+    </row>
+    <row r="1360" spans="1:1">
+      <c r="A1360" s="2"/>
+    </row>
+    <row r="1395" spans="1:1">
+      <c r="A1395" s="2"/>
+    </row>
+    <row r="1396" spans="1:1">
+      <c r="A1396" s="2"/>
+    </row>
+    <row r="1397" spans="1:1">
+      <c r="A1397" s="2"/>
+    </row>
+    <row r="1398" spans="1:1">
+      <c r="A1398" s="2"/>
+    </row>
+    <row r="1399" spans="1:1">
+      <c r="A1399" s="2"/>
+    </row>
+    <row r="1400" spans="1:1">
+      <c r="A1400" s="2"/>
+    </row>
+    <row r="1442" spans="2:4">
+      <c r="C1442" s="2"/>
+      <c r="D1442" s="12"/>
+    </row>
+    <row r="1443" spans="2:4">
+      <c r="B1443" s="2"/>
+      <c r="C1443" s="2"/>
+      <c r="D1443" s="12"/>
+    </row>
+    <row r="1444" spans="2:4">
+      <c r="B1444" s="2"/>
+      <c r="C1444" s="2"/>
+      <c r="D1444" s="12"/>
+    </row>
+    <row r="1445" spans="2:4">
+      <c r="B1445" s="2"/>
+      <c r="C1445" s="2"/>
+      <c r="D1445" s="12"/>
+    </row>
+    <row r="1446" spans="2:4">
+      <c r="C1446" s="2"/>
+      <c r="D1446" s="12"/>
+    </row>
+    <row r="1509" spans="1:1">
+      <c r="A1509" s="2"/>
+    </row>
+    <row r="1510" spans="1:1">
+      <c r="A1510" s="2"/>
+    </row>
+    <row r="1511" spans="1:1">
+      <c r="A1511" s="2"/>
+    </row>
+    <row r="1512" spans="1:1">
+      <c r="A1512" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Creating minimal, systematically named EPV consenus set
</commit_message>
<xml_diff>
--- a/tabular/references/reference_feature_locations.xlsx
+++ b/tabular/references/reference_feature_locations.xlsx
@@ -218,9 +218,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1661">
+  <cellStyleXfs count="1663">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1906,7 +1908,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1661">
+  <cellStyles count="1663">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2738,6 +2740,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1656" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1658" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1662" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -3567,6 +3570,7 @@
     <cellStyle name="Hyperlink" xfId="1655" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1657" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1661" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3903,8 +3907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1512"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D55" sqref="A1:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Corrected feature location on reference for Mus chapparvovirus
</commit_message>
<xml_diff>
--- a/tabular/references/reference_feature_locations.xlsx
+++ b/tabular/references/reference_feature_locations.xlsx
@@ -3908,7 +3908,7 @@
   <dimension ref="A1:E1512"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D55" sqref="A1:D55"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4644,7 +4644,7 @@
         <v>11</v>
       </c>
       <c r="C52" s="5">
-        <v>2109</v>
+        <v>2110</v>
       </c>
       <c r="D52" s="9">
         <v>2728</v>
@@ -4675,7 +4675,7 @@
         <v>2006</v>
       </c>
       <c r="D54" s="9">
-        <v>2726</v>
+        <v>2725</v>
       </c>
     </row>
     <row r="55" spans="1:4">

</xml_diff>